<commit_message>
Checkpoint: funcionando facturas con plantilla y sin plantilla V1
</commit_message>
<xml_diff>
--- a/uploads/processed_template.xlsx
+++ b/uploads/processed_template.xlsx
@@ -504,7 +504,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-08-26</t>
+          <t>26/08/2025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -517,10 +517,8 @@
           <t>3927534</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>001984</t>
-        </is>
+      <c r="D2" t="n">
+        <v>1984</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -535,14 +533,12 @@
           <t>Maria Reyna Guzman Bejarano</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>6255258016</t>
-        </is>
+      <c r="H2" t="n">
+        <v>6255258016</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>En La Esquina Del Hospital Municipal De Cotoca Por La Entrada De Emergencia Rodolfo Añez, Nro.: S/N Zona/Barrio.: COTOCA</t>
+          <t>En La Esquina Del Hospital Municipal De Cotoca Por La Entrada De Emergencia Rodolfo Añez Nro.: S/N Zona/Barrio.: COTOCA</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">

</xml_diff>